<commit_message>
fixed payoffs func and payoffs csv file
</commit_message>
<xml_diff>
--- a/progressivity_pres/payoffs_db_step_5.xlsx
+++ b/progressivity_pres/payoffs_db_step_5.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -443,22 +443,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>10.55</v>
+        <v>9.31</v>
       </c>
       <c r="C3">
-        <v>17.221</v>
+        <v>15.444</v>
       </c>
       <c r="D3">
-        <v>27.893</v>
+        <v>25.579</v>
       </c>
       <c r="E3">
-        <v>43.477</v>
+        <v>40.695</v>
       </c>
       <c r="F3">
-        <v>81.375</v>
+        <v>80.27500000000001</v>
       </c>
       <c r="G3">
-        <v>120.75</v>
+        <v>124.15</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -466,22 +466,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>12.1</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C4">
-        <v>19.441</v>
+        <v>15.888</v>
       </c>
       <c r="D4">
-        <v>30.786</v>
+        <v>26.157</v>
       </c>
       <c r="E4">
-        <v>46.955</v>
+        <v>41.391</v>
       </c>
       <c r="F4">
-        <v>82.75</v>
+        <v>80.55</v>
       </c>
       <c r="G4">
-        <v>116.5</v>
+        <v>123.3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,22 +489,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13.65</v>
+        <v>9.93</v>
       </c>
       <c r="C5">
-        <v>21.662</v>
+        <v>16.332</v>
       </c>
       <c r="D5">
-        <v>33.679</v>
+        <v>26.736</v>
       </c>
       <c r="E5">
-        <v>50.432</v>
+        <v>42.086</v>
       </c>
       <c r="F5">
-        <v>84.125</v>
+        <v>80.825</v>
       </c>
       <c r="G5">
-        <v>112.25</v>
+        <v>122.45</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,22 +512,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>15.2</v>
+        <v>10.24</v>
       </c>
       <c r="C6">
-        <v>23.882</v>
+        <v>16.776</v>
       </c>
       <c r="D6">
-        <v>36.571</v>
+        <v>27.314</v>
       </c>
       <c r="E6">
-        <v>53.909</v>
+        <v>42.782</v>
       </c>
       <c r="F6">
-        <v>85.5</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="G6">
-        <v>108</v>
+        <v>121.6</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -535,22 +535,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>16.75</v>
+        <v>10.55</v>
       </c>
       <c r="C7">
-        <v>26.103</v>
+        <v>17.221</v>
       </c>
       <c r="D7">
-        <v>39.464</v>
+        <v>27.893</v>
       </c>
       <c r="E7">
-        <v>57.386</v>
+        <v>43.477</v>
       </c>
       <c r="F7">
-        <v>86.875</v>
+        <v>81.375</v>
       </c>
       <c r="G7">
-        <v>103.75</v>
+        <v>120.75</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,22 +558,22 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>18.3</v>
+        <v>10.86</v>
       </c>
       <c r="C8">
-        <v>28.324</v>
+        <v>17.665</v>
       </c>
       <c r="D8">
-        <v>42.357</v>
+        <v>28.471</v>
       </c>
       <c r="E8">
-        <v>60.864</v>
+        <v>44.173</v>
       </c>
       <c r="F8">
-        <v>88.25</v>
+        <v>81.65000000000001</v>
       </c>
       <c r="G8">
-        <v>99.5</v>
+        <v>119.9</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -581,22 +581,22 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>19.85</v>
+        <v>11.17</v>
       </c>
       <c r="C9">
-        <v>30.544</v>
+        <v>18.109</v>
       </c>
       <c r="D9">
-        <v>45.25</v>
+        <v>29.05</v>
       </c>
       <c r="E9">
-        <v>64.34099999999999</v>
+        <v>44.868</v>
       </c>
       <c r="F9">
-        <v>89.625</v>
+        <v>81.925</v>
       </c>
       <c r="G9">
-        <v>95.25</v>
+        <v>119.05</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -604,22 +604,22 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>21.4</v>
+        <v>11.48</v>
       </c>
       <c r="C10">
-        <v>32.765</v>
+        <v>18.553</v>
       </c>
       <c r="D10">
-        <v>48.143</v>
+        <v>29.629</v>
       </c>
       <c r="E10">
-        <v>67.818</v>
+        <v>45.564</v>
       </c>
       <c r="F10">
-        <v>91</v>
+        <v>82.2</v>
       </c>
       <c r="G10">
-        <v>91</v>
+        <v>118.2</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -627,22 +627,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>22.95</v>
+        <v>11.79</v>
       </c>
       <c r="C11">
-        <v>34.985</v>
+        <v>18.997</v>
       </c>
       <c r="D11">
-        <v>51.036</v>
+        <v>30.207</v>
       </c>
       <c r="E11">
-        <v>71.295</v>
+        <v>46.259</v>
       </c>
       <c r="F11">
-        <v>92.375</v>
+        <v>82.47499999999999</v>
       </c>
       <c r="G11">
-        <v>86.75</v>
+        <v>117.35</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -650,22 +650,22 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>24.5</v>
+        <v>12.1</v>
       </c>
       <c r="C12">
-        <v>37.206</v>
+        <v>19.441</v>
       </c>
       <c r="D12">
-        <v>53.929</v>
+        <v>30.786</v>
       </c>
       <c r="E12">
-        <v>74.773</v>
+        <v>46.955</v>
       </c>
       <c r="F12">
-        <v>93.75</v>
+        <v>82.75</v>
       </c>
       <c r="G12">
-        <v>82.5</v>
+        <v>116.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -673,22 +673,22 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>26.05</v>
+        <v>12.41</v>
       </c>
       <c r="C13">
-        <v>39.426</v>
+        <v>19.885</v>
       </c>
       <c r="D13">
-        <v>56.821</v>
+        <v>31.364</v>
       </c>
       <c r="E13">
-        <v>78.25</v>
+        <v>47.65</v>
       </c>
       <c r="F13">
-        <v>95.125</v>
+        <v>83.02500000000001</v>
       </c>
       <c r="G13">
-        <v>78.25</v>
+        <v>115.65</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -696,22 +696,22 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>27.6</v>
+        <v>12.72</v>
       </c>
       <c r="C14">
-        <v>41.647</v>
+        <v>20.329</v>
       </c>
       <c r="D14">
-        <v>59.714</v>
+        <v>31.943</v>
       </c>
       <c r="E14">
-        <v>81.727</v>
+        <v>48.345</v>
       </c>
       <c r="F14">
-        <v>96.5</v>
+        <v>83.3</v>
       </c>
       <c r="G14">
-        <v>74</v>
+        <v>114.8</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -719,22 +719,22 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>29.15</v>
+        <v>13.03</v>
       </c>
       <c r="C15">
-        <v>43.868</v>
+        <v>20.774</v>
       </c>
       <c r="D15">
-        <v>62.607</v>
+        <v>32.521</v>
       </c>
       <c r="E15">
-        <v>85.205</v>
+        <v>49.041</v>
       </c>
       <c r="F15">
-        <v>97.875</v>
+        <v>83.575</v>
       </c>
       <c r="G15">
-        <v>69.75</v>
+        <v>113.95</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -742,22 +742,22 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>30.7</v>
+        <v>13.34</v>
       </c>
       <c r="C16">
-        <v>46.088</v>
+        <v>21.218</v>
       </c>
       <c r="D16">
-        <v>65.5</v>
+        <v>33.1</v>
       </c>
       <c r="E16">
-        <v>88.682</v>
+        <v>49.736</v>
       </c>
       <c r="F16">
-        <v>99.25</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="G16">
-        <v>65.5</v>
+        <v>113.1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -765,22 +765,22 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>32.25</v>
+        <v>13.65</v>
       </c>
       <c r="C17">
-        <v>48.309</v>
+        <v>21.662</v>
       </c>
       <c r="D17">
-        <v>68.393</v>
+        <v>33.679</v>
       </c>
       <c r="E17">
-        <v>92.15900000000001</v>
+        <v>50.432</v>
       </c>
       <c r="F17">
-        <v>100.625</v>
+        <v>84.125</v>
       </c>
       <c r="G17">
-        <v>61.25</v>
+        <v>112.25</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -788,22 +788,22 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>33.8</v>
+        <v>13.96</v>
       </c>
       <c r="C18">
-        <v>50.529</v>
+        <v>22.106</v>
       </c>
       <c r="D18">
-        <v>71.286</v>
+        <v>34.257</v>
       </c>
       <c r="E18">
-        <v>95.636</v>
+        <v>51.127</v>
       </c>
       <c r="F18">
-        <v>102</v>
+        <v>84.40000000000001</v>
       </c>
       <c r="G18">
-        <v>57</v>
+        <v>111.4</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -811,22 +811,22 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>35.35</v>
+        <v>14.27</v>
       </c>
       <c r="C19">
-        <v>52.75</v>
+        <v>22.55</v>
       </c>
       <c r="D19">
-        <v>74.179</v>
+        <v>34.836</v>
       </c>
       <c r="E19">
-        <v>99.114</v>
+        <v>51.823</v>
       </c>
       <c r="F19">
-        <v>103.375</v>
+        <v>84.675</v>
       </c>
       <c r="G19">
-        <v>52.75</v>
+        <v>110.55</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -834,22 +834,22 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>36.9</v>
+        <v>14.58</v>
       </c>
       <c r="C20">
-        <v>54.971</v>
+        <v>22.994</v>
       </c>
       <c r="D20">
-        <v>77.071</v>
+        <v>35.414</v>
       </c>
       <c r="E20">
-        <v>102.591</v>
+        <v>52.518</v>
       </c>
       <c r="F20">
-        <v>104.75</v>
+        <v>84.95</v>
       </c>
       <c r="G20">
-        <v>48.5</v>
+        <v>109.7</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -857,22 +857,22 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>38.45</v>
+        <v>14.89</v>
       </c>
       <c r="C21">
-        <v>57.191</v>
+        <v>23.438</v>
       </c>
       <c r="D21">
-        <v>79.964</v>
+        <v>35.993</v>
       </c>
       <c r="E21">
-        <v>106.068</v>
+        <v>53.214</v>
       </c>
       <c r="F21">
-        <v>106.125</v>
+        <v>85.22499999999999</v>
       </c>
       <c r="G21">
-        <v>44.25</v>
+        <v>108.85</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -880,21 +880,1861 @@
         <v>20</v>
       </c>
       <c r="B22">
+        <v>15.2</v>
+      </c>
+      <c r="C22">
+        <v>23.882</v>
+      </c>
+      <c r="D22">
+        <v>36.571</v>
+      </c>
+      <c r="E22">
+        <v>53.909</v>
+      </c>
+      <c r="F22">
+        <v>85.5</v>
+      </c>
+      <c r="G22">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>15.51</v>
+      </c>
+      <c r="C23">
+        <v>24.326</v>
+      </c>
+      <c r="D23">
+        <v>37.15</v>
+      </c>
+      <c r="E23">
+        <v>54.605</v>
+      </c>
+      <c r="F23">
+        <v>85.77500000000001</v>
+      </c>
+      <c r="G23">
+        <v>107.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>15.82</v>
+      </c>
+      <c r="C24">
+        <v>24.771</v>
+      </c>
+      <c r="D24">
+        <v>37.729</v>
+      </c>
+      <c r="E24">
+        <v>55.3</v>
+      </c>
+      <c r="F24">
+        <v>86.05</v>
+      </c>
+      <c r="G24">
+        <v>106.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>16.13</v>
+      </c>
+      <c r="C25">
+        <v>25.215</v>
+      </c>
+      <c r="D25">
+        <v>38.307</v>
+      </c>
+      <c r="E25">
+        <v>55.995</v>
+      </c>
+      <c r="F25">
+        <v>86.325</v>
+      </c>
+      <c r="G25">
+        <v>105.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>16.44</v>
+      </c>
+      <c r="C26">
+        <v>25.659</v>
+      </c>
+      <c r="D26">
+        <v>38.886</v>
+      </c>
+      <c r="E26">
+        <v>56.691</v>
+      </c>
+      <c r="F26">
+        <v>86.59999999999999</v>
+      </c>
+      <c r="G26">
+        <v>104.6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>16.75</v>
+      </c>
+      <c r="C27">
+        <v>26.103</v>
+      </c>
+      <c r="D27">
+        <v>39.464</v>
+      </c>
+      <c r="E27">
+        <v>57.386</v>
+      </c>
+      <c r="F27">
+        <v>86.875</v>
+      </c>
+      <c r="G27">
+        <v>103.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>17.06</v>
+      </c>
+      <c r="C28">
+        <v>26.547</v>
+      </c>
+      <c r="D28">
+        <v>40.043</v>
+      </c>
+      <c r="E28">
+        <v>58.082</v>
+      </c>
+      <c r="F28">
+        <v>87.15000000000001</v>
+      </c>
+      <c r="G28">
+        <v>102.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>17.37</v>
+      </c>
+      <c r="C29">
+        <v>26.991</v>
+      </c>
+      <c r="D29">
+        <v>40.621</v>
+      </c>
+      <c r="E29">
+        <v>58.777</v>
+      </c>
+      <c r="F29">
+        <v>87.425</v>
+      </c>
+      <c r="G29">
+        <v>102.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>17.68</v>
+      </c>
+      <c r="C30">
+        <v>27.435</v>
+      </c>
+      <c r="D30">
+        <v>41.2</v>
+      </c>
+      <c r="E30">
+        <v>59.473</v>
+      </c>
+      <c r="F30">
+        <v>87.7</v>
+      </c>
+      <c r="G30">
+        <v>101.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>17.99</v>
+      </c>
+      <c r="C31">
+        <v>27.879</v>
+      </c>
+      <c r="D31">
+        <v>41.779</v>
+      </c>
+      <c r="E31">
+        <v>60.168</v>
+      </c>
+      <c r="F31">
+        <v>87.97499999999999</v>
+      </c>
+      <c r="G31">
+        <v>100.35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>18.3</v>
+      </c>
+      <c r="C32">
+        <v>28.324</v>
+      </c>
+      <c r="D32">
+        <v>42.357</v>
+      </c>
+      <c r="E32">
+        <v>60.864</v>
+      </c>
+      <c r="F32">
+        <v>88.25</v>
+      </c>
+      <c r="G32">
+        <v>99.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>18.61</v>
+      </c>
+      <c r="C33">
+        <v>28.768</v>
+      </c>
+      <c r="D33">
+        <v>42.936</v>
+      </c>
+      <c r="E33">
+        <v>61.559</v>
+      </c>
+      <c r="F33">
+        <v>88.52500000000001</v>
+      </c>
+      <c r="G33">
+        <v>98.65000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>18.92</v>
+      </c>
+      <c r="C34">
+        <v>29.212</v>
+      </c>
+      <c r="D34">
+        <v>43.514</v>
+      </c>
+      <c r="E34">
+        <v>62.255</v>
+      </c>
+      <c r="F34">
+        <v>88.8</v>
+      </c>
+      <c r="G34">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>19.23</v>
+      </c>
+      <c r="C35">
+        <v>29.656</v>
+      </c>
+      <c r="D35">
+        <v>44.093</v>
+      </c>
+      <c r="E35">
+        <v>62.95</v>
+      </c>
+      <c r="F35">
+        <v>89.075</v>
+      </c>
+      <c r="G35">
+        <v>96.95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>19.54</v>
+      </c>
+      <c r="C36">
+        <v>30.1</v>
+      </c>
+      <c r="D36">
+        <v>44.671</v>
+      </c>
+      <c r="E36">
+        <v>63.645</v>
+      </c>
+      <c r="F36">
+        <v>89.34999999999999</v>
+      </c>
+      <c r="G36">
+        <v>96.09999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>19.85</v>
+      </c>
+      <c r="C37">
+        <v>30.544</v>
+      </c>
+      <c r="D37">
+        <v>45.25</v>
+      </c>
+      <c r="E37">
+        <v>64.34099999999999</v>
+      </c>
+      <c r="F37">
+        <v>89.625</v>
+      </c>
+      <c r="G37">
+        <v>95.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>20.16</v>
+      </c>
+      <c r="C38">
+        <v>30.988</v>
+      </c>
+      <c r="D38">
+        <v>45.829</v>
+      </c>
+      <c r="E38">
+        <v>65.036</v>
+      </c>
+      <c r="F38">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="G38">
+        <v>94.40000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>20.47</v>
+      </c>
+      <c r="C39">
+        <v>31.432</v>
+      </c>
+      <c r="D39">
+        <v>46.407</v>
+      </c>
+      <c r="E39">
+        <v>65.732</v>
+      </c>
+      <c r="F39">
+        <v>90.175</v>
+      </c>
+      <c r="G39">
+        <v>93.55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>20.78</v>
+      </c>
+      <c r="C40">
+        <v>31.876</v>
+      </c>
+      <c r="D40">
+        <v>46.986</v>
+      </c>
+      <c r="E40">
+        <v>66.42700000000001</v>
+      </c>
+      <c r="F40">
+        <v>90.45</v>
+      </c>
+      <c r="G40">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>21.09</v>
+      </c>
+      <c r="C41">
+        <v>32.321</v>
+      </c>
+      <c r="D41">
+        <v>47.564</v>
+      </c>
+      <c r="E41">
+        <v>67.123</v>
+      </c>
+      <c r="F41">
+        <v>90.72499999999999</v>
+      </c>
+      <c r="G41">
+        <v>91.84999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="C22">
+      <c r="B42">
+        <v>21.4</v>
+      </c>
+      <c r="C42">
+        <v>32.765</v>
+      </c>
+      <c r="D42">
+        <v>48.143</v>
+      </c>
+      <c r="E42">
+        <v>67.818</v>
+      </c>
+      <c r="F42">
+        <v>91</v>
+      </c>
+      <c r="G42">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>21.71</v>
+      </c>
+      <c r="C43">
+        <v>33.209</v>
+      </c>
+      <c r="D43">
+        <v>48.721</v>
+      </c>
+      <c r="E43">
+        <v>68.514</v>
+      </c>
+      <c r="F43">
+        <v>91.27500000000001</v>
+      </c>
+      <c r="G43">
+        <v>90.15000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>22.02</v>
+      </c>
+      <c r="C44">
+        <v>33.653</v>
+      </c>
+      <c r="D44">
+        <v>49.3</v>
+      </c>
+      <c r="E44">
+        <v>69.209</v>
+      </c>
+      <c r="F44">
+        <v>91.55</v>
+      </c>
+      <c r="G44">
+        <v>89.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>22.33</v>
+      </c>
+      <c r="C45">
+        <v>34.097</v>
+      </c>
+      <c r="D45">
+        <v>49.879</v>
+      </c>
+      <c r="E45">
+        <v>69.905</v>
+      </c>
+      <c r="F45">
+        <v>91.825</v>
+      </c>
+      <c r="G45">
+        <v>88.45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>22.64</v>
+      </c>
+      <c r="C46">
+        <v>34.541</v>
+      </c>
+      <c r="D46">
+        <v>50.457</v>
+      </c>
+      <c r="E46">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="F46">
+        <v>92.09999999999999</v>
+      </c>
+      <c r="G46">
+        <v>87.59999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>22.95</v>
+      </c>
+      <c r="C47">
+        <v>34.985</v>
+      </c>
+      <c r="D47">
+        <v>51.036</v>
+      </c>
+      <c r="E47">
+        <v>71.295</v>
+      </c>
+      <c r="F47">
+        <v>92.375</v>
+      </c>
+      <c r="G47">
+        <v>86.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>23.26</v>
+      </c>
+      <c r="C48">
+        <v>35.429</v>
+      </c>
+      <c r="D48">
+        <v>51.614</v>
+      </c>
+      <c r="E48">
+        <v>71.991</v>
+      </c>
+      <c r="F48">
+        <v>92.65000000000001</v>
+      </c>
+      <c r="G48">
+        <v>85.90000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>23.57</v>
+      </c>
+      <c r="C49">
+        <v>35.874</v>
+      </c>
+      <c r="D49">
+        <v>52.193</v>
+      </c>
+      <c r="E49">
+        <v>72.68600000000001</v>
+      </c>
+      <c r="F49">
+        <v>92.925</v>
+      </c>
+      <c r="G49">
+        <v>85.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>23.88</v>
+      </c>
+      <c r="C50">
+        <v>36.318</v>
+      </c>
+      <c r="D50">
+        <v>52.771</v>
+      </c>
+      <c r="E50">
+        <v>73.38200000000001</v>
+      </c>
+      <c r="F50">
+        <v>93.2</v>
+      </c>
+      <c r="G50">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>24.19</v>
+      </c>
+      <c r="C51">
+        <v>36.762</v>
+      </c>
+      <c r="D51">
+        <v>53.35</v>
+      </c>
+      <c r="E51">
+        <v>74.077</v>
+      </c>
+      <c r="F51">
+        <v>93.47499999999999</v>
+      </c>
+      <c r="G51">
+        <v>83.34999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>24.5</v>
+      </c>
+      <c r="C52">
+        <v>37.206</v>
+      </c>
+      <c r="D52">
+        <v>53.929</v>
+      </c>
+      <c r="E52">
+        <v>74.773</v>
+      </c>
+      <c r="F52">
+        <v>93.75</v>
+      </c>
+      <c r="G52">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>24.81</v>
+      </c>
+      <c r="C53">
+        <v>37.65</v>
+      </c>
+      <c r="D53">
+        <v>54.507</v>
+      </c>
+      <c r="E53">
+        <v>75.468</v>
+      </c>
+      <c r="F53">
+        <v>94.02500000000001</v>
+      </c>
+      <c r="G53">
+        <v>81.65000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>25.12</v>
+      </c>
+      <c r="C54">
+        <v>38.094</v>
+      </c>
+      <c r="D54">
+        <v>55.086</v>
+      </c>
+      <c r="E54">
+        <v>76.164</v>
+      </c>
+      <c r="F54">
+        <v>94.3</v>
+      </c>
+      <c r="G54">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>25.43</v>
+      </c>
+      <c r="C55">
+        <v>38.538</v>
+      </c>
+      <c r="D55">
+        <v>55.664</v>
+      </c>
+      <c r="E55">
+        <v>76.85899999999999</v>
+      </c>
+      <c r="F55">
+        <v>94.575</v>
+      </c>
+      <c r="G55">
+        <v>79.95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>25.74</v>
+      </c>
+      <c r="C56">
+        <v>38.982</v>
+      </c>
+      <c r="D56">
+        <v>56.243</v>
+      </c>
+      <c r="E56">
+        <v>77.55500000000001</v>
+      </c>
+      <c r="F56">
+        <v>94.84999999999999</v>
+      </c>
+      <c r="G56">
+        <v>79.09999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>26.05</v>
+      </c>
+      <c r="C57">
+        <v>39.426</v>
+      </c>
+      <c r="D57">
+        <v>56.821</v>
+      </c>
+      <c r="E57">
+        <v>78.25</v>
+      </c>
+      <c r="F57">
+        <v>95.125</v>
+      </c>
+      <c r="G57">
+        <v>78.25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>26.36</v>
+      </c>
+      <c r="C58">
+        <v>39.871</v>
+      </c>
+      <c r="D58">
+        <v>57.4</v>
+      </c>
+      <c r="E58">
+        <v>78.94499999999999</v>
+      </c>
+      <c r="F58">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="G58">
+        <v>77.40000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>26.67</v>
+      </c>
+      <c r="C59">
+        <v>40.315</v>
+      </c>
+      <c r="D59">
+        <v>57.979</v>
+      </c>
+      <c r="E59">
+        <v>79.64100000000001</v>
+      </c>
+      <c r="F59">
+        <v>95.675</v>
+      </c>
+      <c r="G59">
+        <v>76.55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>26.98</v>
+      </c>
+      <c r="C60">
+        <v>40.759</v>
+      </c>
+      <c r="D60">
+        <v>58.557</v>
+      </c>
+      <c r="E60">
+        <v>80.336</v>
+      </c>
+      <c r="F60">
+        <v>95.95</v>
+      </c>
+      <c r="G60">
+        <v>75.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>27.29</v>
+      </c>
+      <c r="C61">
+        <v>41.203</v>
+      </c>
+      <c r="D61">
+        <v>59.136</v>
+      </c>
+      <c r="E61">
+        <v>81.032</v>
+      </c>
+      <c r="F61">
+        <v>96.22499999999999</v>
+      </c>
+      <c r="G61">
+        <v>74.84999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>27.6</v>
+      </c>
+      <c r="C62">
+        <v>41.647</v>
+      </c>
+      <c r="D62">
+        <v>59.714</v>
+      </c>
+      <c r="E62">
+        <v>81.727</v>
+      </c>
+      <c r="F62">
+        <v>96.5</v>
+      </c>
+      <c r="G62">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>27.91</v>
+      </c>
+      <c r="C63">
+        <v>42.091</v>
+      </c>
+      <c r="D63">
+        <v>60.293</v>
+      </c>
+      <c r="E63">
+        <v>82.423</v>
+      </c>
+      <c r="F63">
+        <v>96.77500000000001</v>
+      </c>
+      <c r="G63">
+        <v>73.15000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>28.22</v>
+      </c>
+      <c r="C64">
+        <v>42.535</v>
+      </c>
+      <c r="D64">
+        <v>60.871</v>
+      </c>
+      <c r="E64">
+        <v>83.11799999999999</v>
+      </c>
+      <c r="F64">
+        <v>97.05</v>
+      </c>
+      <c r="G64">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>28.53</v>
+      </c>
+      <c r="C65">
+        <v>42.979</v>
+      </c>
+      <c r="D65">
+        <v>61.45</v>
+      </c>
+      <c r="E65">
+        <v>83.81399999999999</v>
+      </c>
+      <c r="F65">
+        <v>97.325</v>
+      </c>
+      <c r="G65">
+        <v>71.45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>28.84</v>
+      </c>
+      <c r="C66">
+        <v>43.424</v>
+      </c>
+      <c r="D66">
+        <v>62.029</v>
+      </c>
+      <c r="E66">
+        <v>84.509</v>
+      </c>
+      <c r="F66">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="G66">
+        <v>70.59999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>29.15</v>
+      </c>
+      <c r="C67">
+        <v>43.868</v>
+      </c>
+      <c r="D67">
+        <v>62.607</v>
+      </c>
+      <c r="E67">
+        <v>85.205</v>
+      </c>
+      <c r="F67">
+        <v>97.875</v>
+      </c>
+      <c r="G67">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>29.46</v>
+      </c>
+      <c r="C68">
+        <v>44.312</v>
+      </c>
+      <c r="D68">
+        <v>63.186</v>
+      </c>
+      <c r="E68">
+        <v>85.90000000000001</v>
+      </c>
+      <c r="F68">
+        <v>98.15000000000001</v>
+      </c>
+      <c r="G68">
+        <v>68.90000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>29.77</v>
+      </c>
+      <c r="C69">
+        <v>44.756</v>
+      </c>
+      <c r="D69">
+        <v>63.764</v>
+      </c>
+      <c r="E69">
+        <v>86.595</v>
+      </c>
+      <c r="F69">
+        <v>98.425</v>
+      </c>
+      <c r="G69">
+        <v>68.05</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>30.08</v>
+      </c>
+      <c r="C70">
+        <v>45.2</v>
+      </c>
+      <c r="D70">
+        <v>64.343</v>
+      </c>
+      <c r="E70">
+        <v>87.291</v>
+      </c>
+      <c r="F70">
+        <v>98.7</v>
+      </c>
+      <c r="G70">
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>30.39</v>
+      </c>
+      <c r="C71">
+        <v>45.644</v>
+      </c>
+      <c r="D71">
+        <v>64.92100000000001</v>
+      </c>
+      <c r="E71">
+        <v>87.986</v>
+      </c>
+      <c r="F71">
+        <v>98.97499999999999</v>
+      </c>
+      <c r="G71">
+        <v>66.34999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>30.7</v>
+      </c>
+      <c r="C72">
+        <v>46.088</v>
+      </c>
+      <c r="D72">
+        <v>65.5</v>
+      </c>
+      <c r="E72">
+        <v>88.682</v>
+      </c>
+      <c r="F72">
+        <v>99.25</v>
+      </c>
+      <c r="G72">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>31.01</v>
+      </c>
+      <c r="C73">
+        <v>46.532</v>
+      </c>
+      <c r="D73">
+        <v>66.07899999999999</v>
+      </c>
+      <c r="E73">
+        <v>89.377</v>
+      </c>
+      <c r="F73">
+        <v>99.52500000000001</v>
+      </c>
+      <c r="G73">
+        <v>64.65000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>31.32</v>
+      </c>
+      <c r="C74">
+        <v>46.976</v>
+      </c>
+      <c r="D74">
+        <v>66.657</v>
+      </c>
+      <c r="E74">
+        <v>90.07299999999999</v>
+      </c>
+      <c r="F74">
+        <v>99.8</v>
+      </c>
+      <c r="G74">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>31.63</v>
+      </c>
+      <c r="C75">
+        <v>47.421</v>
+      </c>
+      <c r="D75">
+        <v>67.236</v>
+      </c>
+      <c r="E75">
+        <v>90.768</v>
+      </c>
+      <c r="F75">
+        <v>100.075</v>
+      </c>
+      <c r="G75">
+        <v>62.95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>31.94</v>
+      </c>
+      <c r="C76">
+        <v>47.865</v>
+      </c>
+      <c r="D76">
+        <v>67.81399999999999</v>
+      </c>
+      <c r="E76">
+        <v>91.464</v>
+      </c>
+      <c r="F76">
+        <v>100.35</v>
+      </c>
+      <c r="G76">
+        <v>62.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>32.25</v>
+      </c>
+      <c r="C77">
+        <v>48.309</v>
+      </c>
+      <c r="D77">
+        <v>68.393</v>
+      </c>
+      <c r="E77">
+        <v>92.15900000000001</v>
+      </c>
+      <c r="F77">
+        <v>100.625</v>
+      </c>
+      <c r="G77">
+        <v>61.25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>32.56</v>
+      </c>
+      <c r="C78">
+        <v>48.753</v>
+      </c>
+      <c r="D78">
+        <v>68.971</v>
+      </c>
+      <c r="E78">
+        <v>92.855</v>
+      </c>
+      <c r="F78">
+        <v>100.9</v>
+      </c>
+      <c r="G78">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>32.87</v>
+      </c>
+      <c r="C79">
+        <v>49.197</v>
+      </c>
+      <c r="D79">
+        <v>69.55</v>
+      </c>
+      <c r="E79">
+        <v>93.55</v>
+      </c>
+      <c r="F79">
+        <v>101.175</v>
+      </c>
+      <c r="G79">
+        <v>59.55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>33.18</v>
+      </c>
+      <c r="C80">
+        <v>49.641</v>
+      </c>
+      <c r="D80">
+        <v>70.129</v>
+      </c>
+      <c r="E80">
+        <v>94.245</v>
+      </c>
+      <c r="F80">
+        <v>101.45</v>
+      </c>
+      <c r="G80">
+        <v>58.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>33.49</v>
+      </c>
+      <c r="C81">
+        <v>50.085</v>
+      </c>
+      <c r="D81">
+        <v>70.70699999999999</v>
+      </c>
+      <c r="E81">
+        <v>94.941</v>
+      </c>
+      <c r="F81">
+        <v>101.725</v>
+      </c>
+      <c r="G81">
+        <v>57.85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>33.8</v>
+      </c>
+      <c r="C82">
+        <v>50.529</v>
+      </c>
+      <c r="D82">
+        <v>71.286</v>
+      </c>
+      <c r="E82">
+        <v>95.636</v>
+      </c>
+      <c r="F82">
+        <v>102</v>
+      </c>
+      <c r="G82">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>34.11</v>
+      </c>
+      <c r="C83">
+        <v>50.974</v>
+      </c>
+      <c r="D83">
+        <v>71.864</v>
+      </c>
+      <c r="E83">
+        <v>96.33199999999999</v>
+      </c>
+      <c r="F83">
+        <v>102.275</v>
+      </c>
+      <c r="G83">
+        <v>56.15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>34.42</v>
+      </c>
+      <c r="C84">
+        <v>51.418</v>
+      </c>
+      <c r="D84">
+        <v>72.443</v>
+      </c>
+      <c r="E84">
+        <v>97.027</v>
+      </c>
+      <c r="F84">
+        <v>102.55</v>
+      </c>
+      <c r="G84">
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>34.73</v>
+      </c>
+      <c r="C85">
+        <v>51.862</v>
+      </c>
+      <c r="D85">
+        <v>73.021</v>
+      </c>
+      <c r="E85">
+        <v>97.723</v>
+      </c>
+      <c r="F85">
+        <v>102.825</v>
+      </c>
+      <c r="G85">
+        <v>54.45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>35.04</v>
+      </c>
+      <c r="C86">
+        <v>52.306</v>
+      </c>
+      <c r="D86">
+        <v>73.59999999999999</v>
+      </c>
+      <c r="E86">
+        <v>98.41800000000001</v>
+      </c>
+      <c r="F86">
+        <v>103.1</v>
+      </c>
+      <c r="G86">
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>35.35</v>
+      </c>
+      <c r="C87">
+        <v>52.75</v>
+      </c>
+      <c r="D87">
+        <v>74.179</v>
+      </c>
+      <c r="E87">
+        <v>99.114</v>
+      </c>
+      <c r="F87">
+        <v>103.375</v>
+      </c>
+      <c r="G87">
+        <v>52.75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>35.66</v>
+      </c>
+      <c r="C88">
+        <v>53.194</v>
+      </c>
+      <c r="D88">
+        <v>74.75700000000001</v>
+      </c>
+      <c r="E88">
+        <v>99.809</v>
+      </c>
+      <c r="F88">
+        <v>103.65</v>
+      </c>
+      <c r="G88">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>35.97</v>
+      </c>
+      <c r="C89">
+        <v>53.638</v>
+      </c>
+      <c r="D89">
+        <v>75.336</v>
+      </c>
+      <c r="E89">
+        <v>100.505</v>
+      </c>
+      <c r="F89">
+        <v>103.925</v>
+      </c>
+      <c r="G89">
+        <v>51.05</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>36.28</v>
+      </c>
+      <c r="C90">
+        <v>54.082</v>
+      </c>
+      <c r="D90">
+        <v>75.914</v>
+      </c>
+      <c r="E90">
+        <v>101.2</v>
+      </c>
+      <c r="F90">
+        <v>104.2</v>
+      </c>
+      <c r="G90">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>36.59</v>
+      </c>
+      <c r="C91">
+        <v>54.526</v>
+      </c>
+      <c r="D91">
+        <v>76.49299999999999</v>
+      </c>
+      <c r="E91">
+        <v>101.895</v>
+      </c>
+      <c r="F91">
+        <v>104.475</v>
+      </c>
+      <c r="G91">
+        <v>49.35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>36.9</v>
+      </c>
+      <c r="C92">
+        <v>54.971</v>
+      </c>
+      <c r="D92">
+        <v>77.071</v>
+      </c>
+      <c r="E92">
+        <v>102.591</v>
+      </c>
+      <c r="F92">
+        <v>104.75</v>
+      </c>
+      <c r="G92">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>37.21</v>
+      </c>
+      <c r="C93">
+        <v>55.415</v>
+      </c>
+      <c r="D93">
+        <v>77.65000000000001</v>
+      </c>
+      <c r="E93">
+        <v>103.286</v>
+      </c>
+      <c r="F93">
+        <v>105.025</v>
+      </c>
+      <c r="G93">
+        <v>47.65</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>37.52</v>
+      </c>
+      <c r="C94">
+        <v>55.859</v>
+      </c>
+      <c r="D94">
+        <v>78.229</v>
+      </c>
+      <c r="E94">
+        <v>103.982</v>
+      </c>
+      <c r="F94">
+        <v>105.3</v>
+      </c>
+      <c r="G94">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>37.83</v>
+      </c>
+      <c r="C95">
+        <v>56.303</v>
+      </c>
+      <c r="D95">
+        <v>78.807</v>
+      </c>
+      <c r="E95">
+        <v>104.677</v>
+      </c>
+      <c r="F95">
+        <v>105.575</v>
+      </c>
+      <c r="G95">
+        <v>45.95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>38.14</v>
+      </c>
+      <c r="C96">
+        <v>56.747</v>
+      </c>
+      <c r="D96">
+        <v>79.386</v>
+      </c>
+      <c r="E96">
+        <v>105.373</v>
+      </c>
+      <c r="F96">
+        <v>105.85</v>
+      </c>
+      <c r="G96">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>38.45</v>
+      </c>
+      <c r="C97">
+        <v>57.191</v>
+      </c>
+      <c r="D97">
+        <v>79.964</v>
+      </c>
+      <c r="E97">
+        <v>106.068</v>
+      </c>
+      <c r="F97">
+        <v>106.125</v>
+      </c>
+      <c r="G97">
+        <v>44.25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>38.76</v>
+      </c>
+      <c r="C98">
+        <v>57.635</v>
+      </c>
+      <c r="D98">
+        <v>80.54300000000001</v>
+      </c>
+      <c r="E98">
+        <v>106.764</v>
+      </c>
+      <c r="F98">
+        <v>106.4</v>
+      </c>
+      <c r="G98">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>39.07</v>
+      </c>
+      <c r="C99">
+        <v>58.079</v>
+      </c>
+      <c r="D99">
+        <v>81.121</v>
+      </c>
+      <c r="E99">
+        <v>107.459</v>
+      </c>
+      <c r="F99">
+        <v>106.675</v>
+      </c>
+      <c r="G99">
+        <v>42.55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>39.38</v>
+      </c>
+      <c r="C100">
+        <v>58.524</v>
+      </c>
+      <c r="D100">
+        <v>81.7</v>
+      </c>
+      <c r="E100">
+        <v>108.155</v>
+      </c>
+      <c r="F100">
+        <v>106.95</v>
+      </c>
+      <c r="G100">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>39.69</v>
+      </c>
+      <c r="C101">
+        <v>58.968</v>
+      </c>
+      <c r="D101">
+        <v>82.279</v>
+      </c>
+      <c r="E101">
+        <v>108.85</v>
+      </c>
+      <c r="F101">
+        <v>107.225</v>
+      </c>
+      <c r="G101">
+        <v>40.85</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>40</v>
+      </c>
+      <c r="C102">
         <v>59.412</v>
       </c>
-      <c r="D22">
+      <c r="D102">
         <v>82.857</v>
       </c>
-      <c r="E22">
+      <c r="E102">
         <v>109.545</v>
       </c>
-      <c r="F22">
+      <c r="F102">
         <v>107.5</v>
       </c>
-      <c r="G22">
+      <c r="G102">
         <v>40</v>
       </c>
     </row>

</xml_diff>